<commit_message>
Copying incorect items, but it is copying somehting. There us an issue with the items
</commit_message>
<xml_diff>
--- a/Examples/mjdexample.xlsx
+++ b/Examples/mjdexample.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hzlan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Desktop\Excel_Combine_And_Sort\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417D5886-8BEA-4D8D-AEAF-77AECB106818}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6850" xr2:uid="{6B9DE2EC-650A-432A-8DAB-1F28E47B9552}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6855"/>
   </bookViews>
   <sheets>
-    <sheet name="DataImReadingIn" sheetId="1" r:id="rId1"/>
+    <sheet name="dces" sheetId="1" r:id="rId1"/>
+    <sheet name="downlinks" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -420,213 +420,249 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19EF48B1-DFEF-4FDD-ABC1-B2D61AD62407}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="O1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="F2">
         <v>22</v>
       </c>
-      <c r="C2" t="s">
+      <c r="O2" t="s">
         <v>2</v>
       </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>23</v>
-      </c>
-      <c r="F2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>6</v>
       </c>
-      <c r="B3">
+      <c r="F3">
         <v>34</v>
       </c>
-      <c r="C3" t="s">
+      <c r="O3" t="s">
         <v>3</v>
       </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3">
-        <v>43</v>
-      </c>
-      <c r="F3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
-      <c r="B4">
+      <c r="F4">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="O4" t="s">
         <v>4</v>
       </c>
-      <c r="D4">
-        <v>9</v>
-      </c>
-      <c r="E4">
-        <v>564</v>
-      </c>
-      <c r="F4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="F5">
         <v>63</v>
       </c>
-      <c r="C5" t="s">
+      <c r="O5" t="s">
         <v>5</v>
       </c>
-      <c r="D5">
-        <v>7</v>
-      </c>
-      <c r="E5">
-        <v>453</v>
-      </c>
-      <c r="F5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>7</v>
       </c>
-      <c r="B6">
+      <c r="F6">
         <v>234</v>
       </c>
-      <c r="C6" t="s">
+      <c r="O6" t="s">
         <v>6</v>
       </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
-      <c r="E6">
-        <v>23</v>
-      </c>
-      <c r="F6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>34</v>
       </c>
-      <c r="B7">
+      <c r="F7">
         <v>45</v>
       </c>
-      <c r="C7" t="s">
+      <c r="O7" t="s">
         <v>7</v>
       </c>
-      <c r="D7">
-        <v>12</v>
-      </c>
-      <c r="E7">
-        <v>6</v>
-      </c>
-      <c r="F7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>35</v>
       </c>
-      <c r="B8">
+      <c r="F8">
         <v>56</v>
       </c>
-      <c r="C8" t="s">
+      <c r="O8" t="s">
         <v>8</v>
       </c>
-      <c r="D8">
-        <v>77</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="F8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="F9">
         <v>76</v>
       </c>
-      <c r="C9" t="s">
+      <c r="O9" t="s">
         <v>9</v>
       </c>
-      <c r="D9">
-        <v>56</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>78</v>
       </c>
-      <c r="B10">
+      <c r="F10">
         <v>45</v>
       </c>
-      <c r="C10" t="s">
+      <c r="O10" t="s">
         <v>10</v>
       </c>
-      <c r="D10">
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>43</v>
+      </c>
+      <c r="G3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>564</v>
+      </c>
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>453</v>
+      </c>
+      <c r="G5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="G7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>77</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>56</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>45</v>
       </c>
-      <c r="E10">
+      <c r="C10">
         <v>4</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>